<commit_message>
Added part links to controller, created BOM for controller
</commit_message>
<xml_diff>
--- a/Controller_PartsList.xlsx
+++ b/Controller_PartsList.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdiro\Desktop\NixieClockRev2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdiro\Desktop\NixieTubeClock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC7D3F0-7A05-4991-A34F-60BE23A07191}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B2C0E8-E939-4DFD-A173-2795DDB788C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25125" yWindow="5040" windowWidth="26460" windowHeight="13860" xr2:uid="{9419127E-C365-4B28-B0E7-0B6ADC239E75}"/>
+    <workbookView xWindow="-14190" yWindow="6375" windowWidth="26460" windowHeight="13860" xr2:uid="{9419127E-C365-4B28-B0E7-0B6ADC239E75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BF1A60-FEC9-436F-950B-2374E06DEF01}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>